<commit_message>
Version 2.0 old blueprints
</commit_message>
<xml_diff>
--- a/Спецификация.xlsx
+++ b/Спецификация.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Учёба\Сушилка\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A692428-4D7C-4D3D-A07C-C87FD1097900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E306D099-013C-4A76-85A2-1E4419528D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="2700" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Поз.</t>
   </si>
@@ -108,13 +108,67 @@
     <t>Валик</t>
   </si>
   <si>
-    <t>Ось</t>
-  </si>
-  <si>
-    <t>Дверца</t>
-  </si>
-  <si>
-    <t>Вентиляция</t>
+    <t>Задняя внутренняя грань</t>
+  </si>
+  <si>
+    <t>Боковая внутренняя грань</t>
+  </si>
+  <si>
+    <t>СК.000.014</t>
+  </si>
+  <si>
+    <t>Вентиляция М2</t>
+  </si>
+  <si>
+    <t>Слот для экрана</t>
+  </si>
+  <si>
+    <t>СК.000.015</t>
+  </si>
+  <si>
+    <t>Ручка</t>
+  </si>
+  <si>
+    <t>СК.000.016</t>
+  </si>
+  <si>
+    <t>Дверца 2.0</t>
+  </si>
+  <si>
+    <t>Окно дверцы</t>
+  </si>
+  <si>
+    <t>СК.000.017</t>
+  </si>
+  <si>
+    <t>Площадь, мм^2</t>
+  </si>
+  <si>
+    <t>Длина реза, мм</t>
+  </si>
+  <si>
+    <t>Итоговая площадь, мм^2</t>
+  </si>
+  <si>
+    <t>Итоговая длина реза, мм</t>
+  </si>
+  <si>
+    <t>Материал</t>
+  </si>
+  <si>
+    <t>Сталь 1 мм</t>
+  </si>
+  <si>
+    <t>Латунь</t>
+  </si>
+  <si>
+    <t>3д печать</t>
+  </si>
+  <si>
+    <t>Орг. Стекло</t>
+  </si>
+  <si>
+    <t>Итого металл:</t>
   </si>
 </sst>
 </file>
@@ -153,13 +207,13 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -441,212 +495,593 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="19.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="3"/>
+    <col min="5" max="5" width="11.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15" style="3" customWidth="1"/>
+    <col min="7" max="7" width="16.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="2">
+        <v>27892.86</v>
+      </c>
+      <c r="G2" s="2">
+        <v>865.56</v>
+      </c>
+      <c r="H2" s="3">
+        <f>F2*D2</f>
+        <v>27892.86</v>
+      </c>
+      <c r="I2" s="3">
+        <f>D2*G2</f>
+        <v>865.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="2">
+        <v>27902.68</v>
+      </c>
+      <c r="G3" s="2">
+        <v>849.86</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H18" si="0">F3*D3</f>
+        <v>27902.68</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ref="I3:I18" si="1">D3*G3</f>
+        <v>849.86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="2">
+        <v>27902.68</v>
+      </c>
+      <c r="G4" s="2">
+        <v>849.86</v>
+      </c>
+      <c r="H4" s="3">
+        <f t="shared" si="0"/>
+        <v>27902.68</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="1"/>
+        <v>849.86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="2">
+        <v>27912.49</v>
+      </c>
+      <c r="G5" s="2">
+        <v>834.15</v>
+      </c>
+      <c r="H5" s="3">
+        <f t="shared" si="0"/>
+        <v>27912.49</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="1"/>
+        <v>834.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+      <c r="E6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="2">
+        <v>74560.58</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2325.48</v>
+      </c>
+      <c r="H6" s="3">
+        <f t="shared" si="0"/>
+        <v>149121.16</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>4650.96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="2">
+        <v>85521.94</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1579.26</v>
+      </c>
+      <c r="H7" s="3">
+        <f t="shared" si="0"/>
+        <v>85521.94</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>1579.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2">
+        <v>85737</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1308.74</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>85737</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="1"/>
+        <v>1308.74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="2">
+        <v>91262.3</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1245.21</v>
+      </c>
+      <c r="H9" s="3">
+        <f t="shared" si="0"/>
+        <v>91262.3</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>1245.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="2">
+        <v>100586.95</v>
+      </c>
+      <c r="G10" s="2">
+        <v>2644.58</v>
+      </c>
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>100586.95</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>2644.58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0</v>
+      </c>
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="D12" s="2">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="2">
+        <v>43677</v>
+      </c>
+      <c r="G12" s="2">
+        <v>909.94</v>
+      </c>
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>43677</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>909.94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="2">
+        <v>38600.53</v>
+      </c>
+      <c r="G13" s="2">
+        <v>906.49</v>
+      </c>
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>77201.06</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>1812.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0</v>
+      </c>
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D14">
-        <v>1</v>
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="2">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="2">
+        <v>1</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="2">
+        <v>43560</v>
+      </c>
+      <c r="G18" s="2">
+        <v>836</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" si="0"/>
+        <v>87120</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="1"/>
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="3">
+        <f>SUM(H2:H13)</f>
+        <v>744718.11999999988</v>
+      </c>
+      <c r="I19" s="3">
+        <f>SUM(I2:I13)</f>
+        <v>17551.099999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>